<commit_message>
Update test of the libraries. Add test to integration test of TableReader.ClosedXML.dll and TableReader.ExcelDataReader.dll. Update the test codes and datas for the libraries above. Fix bugs found while the test of TableReader.ExcelDataReader.dll.
Add description about methods in the TableReader.ClosedXML.ExcelTableReader class.

Change the version of the libraries.
</commit_message>
<xml_diff>
--- a/TableReader/src/test/TestData/TableReader.ClosedXML.Reader_Test.xlsx
+++ b/TableReader/src/test/TestData/TableReader.ClosedXML.Reader_Test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="96">
   <si>
     <t>Header_r_001_c_001</t>
     <phoneticPr fontId="1"/>
@@ -137,6 +137,203 @@
   </si>
   <si>
     <t>Header_003_r_001_c_005</t>
+  </si>
+  <si>
+    <t>TestTable_004</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Header_004_r_001_c_001</t>
+  </si>
+  <si>
+    <t>Header_004_r_001_c_002</t>
+  </si>
+  <si>
+    <t>Header_004_r_001_c_003</t>
+  </si>
+  <si>
+    <t>Header_004_r_001_c_004</t>
+  </si>
+  <si>
+    <t>Data_004_r_001_c_001</t>
+  </si>
+  <si>
+    <t>Data_004_r_001_c_002</t>
+  </si>
+  <si>
+    <t>Data_004_r_001_c_003</t>
+  </si>
+  <si>
+    <t>Data_004_r_001_c_004</t>
+  </si>
+  <si>
+    <t>Data_004_r_001_c_005</t>
+  </si>
+  <si>
+    <t>Data_004_r_002_c_001</t>
+  </si>
+  <si>
+    <t>Data_004_r_002_c_002</t>
+  </si>
+  <si>
+    <t>Data_004_r_002_c_003</t>
+  </si>
+  <si>
+    <t>Data_004_r_002_c_004</t>
+  </si>
+  <si>
+    <t>Data_004_r_002_c_005</t>
+  </si>
+  <si>
+    <t>Data_004_r_003_c_001</t>
+  </si>
+  <si>
+    <t>Data_004_r_003_c_002</t>
+  </si>
+  <si>
+    <t>Data_004_r_003_c_003</t>
+  </si>
+  <si>
+    <t>Data_004_r_003_c_004</t>
+  </si>
+  <si>
+    <t>Data_004_r_003_c_005</t>
+  </si>
+  <si>
+    <t>Data_004_r_004_c_001</t>
+  </si>
+  <si>
+    <t>Data_004_r_004_c_002</t>
+  </si>
+  <si>
+    <t>Data_004_r_004_c_003</t>
+  </si>
+  <si>
+    <t>Data_004_r_004_c_004</t>
+  </si>
+  <si>
+    <t>Data_004_r_004_c_005</t>
+  </si>
+  <si>
+    <t>TestTable_005</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Header_005_r_001_c_001</t>
+  </si>
+  <si>
+    <t>Header_005_r_001_c_002</t>
+  </si>
+  <si>
+    <t>Header_005_r_001_c_003</t>
+  </si>
+  <si>
+    <t>Header_005_r_001_c_004</t>
+  </si>
+  <si>
+    <t>Data_005_r_001_c_002</t>
+  </si>
+  <si>
+    <t>Data_005_r_001_c_003</t>
+  </si>
+  <si>
+    <t>Data_005_r_001_c_004</t>
+  </si>
+  <si>
+    <t>Data_005_r_001_c_005</t>
+  </si>
+  <si>
+    <t>Data_005_r_002_c_001</t>
+  </si>
+  <si>
+    <t>Data_005_r_002_c_002</t>
+  </si>
+  <si>
+    <t>Data_005_r_002_c_003</t>
+  </si>
+  <si>
+    <t>Data_005_r_002_c_004</t>
+  </si>
+  <si>
+    <t>Data_005_r_002_c_005</t>
+  </si>
+  <si>
+    <t>Data_005_r_003_c_001</t>
+  </si>
+  <si>
+    <t>Data_005_r_003_c_002</t>
+  </si>
+  <si>
+    <t>Data_005_r_003_c_003</t>
+  </si>
+  <si>
+    <t>Data_005_r_003_c_004</t>
+  </si>
+  <si>
+    <t>Data_005_r_003_c_005</t>
+  </si>
+  <si>
+    <t>Data_005_r_004_c_001</t>
+  </si>
+  <si>
+    <t>Data_005_r_004_c_002</t>
+  </si>
+  <si>
+    <t>Data_005_r_004_c_003</t>
+  </si>
+  <si>
+    <t>Data_005_r_004_c_004</t>
+  </si>
+  <si>
+    <t>Data_005_r_004_c_005</t>
+  </si>
+  <si>
+    <t>Header_005_r_001_c_005</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TestTable_006</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data_005_r_002_c_001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data_005_r_001_c_001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TestTable_007</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TestTable_008</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data_005_r_003_c_001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data_005_r_004_c_001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data_005_r_001_c_005</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TestTable_009</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data_005_r_003_c_005</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data_005_r_004_c_005</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -464,11 +661,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G16"/>
+  <dimension ref="B2:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -610,6 +805,528 @@
         <v>29</v>
       </c>
     </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" t="s">
+        <v>72</v>
+      </c>
+      <c r="G33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" t="s">
+        <v>82</v>
+      </c>
+      <c r="G35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" t="s">
+        <v>63</v>
+      </c>
+      <c r="F37" t="s">
+        <v>64</v>
+      </c>
+      <c r="G37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" t="s">
+        <v>72</v>
+      </c>
+      <c r="G39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40" t="s">
+        <v>77</v>
+      </c>
+      <c r="G40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" t="s">
+        <v>82</v>
+      </c>
+      <c r="G41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" t="s">
+        <v>63</v>
+      </c>
+      <c r="F43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" t="s">
+        <v>66</v>
+      </c>
+      <c r="F44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" t="s">
+        <v>72</v>
+      </c>
+      <c r="G45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46" t="s">
+        <v>76</v>
+      </c>
+      <c r="F46" t="s">
+        <v>77</v>
+      </c>
+      <c r="G46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" t="s">
+        <v>64</v>
+      </c>
+      <c r="G49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" t="s">
+        <v>66</v>
+      </c>
+      <c r="F50" t="s">
+        <v>67</v>
+      </c>
+      <c r="G50" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" t="s">
+        <v>70</v>
+      </c>
+      <c r="F51" t="s">
+        <v>72</v>
+      </c>
+      <c r="G51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" t="s">
+        <v>75</v>
+      </c>
+      <c r="E52" t="s">
+        <v>76</v>
+      </c>
+      <c r="F52" t="s">
+        <v>77</v>
+      </c>
+      <c r="G52" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" t="s">
+        <v>80</v>
+      </c>
+      <c r="E53" t="s">
+        <v>81</v>
+      </c>
+      <c r="F53" t="s">
+        <v>82</v>
+      </c>
+      <c r="G53" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>